<commit_message>
I correct the extracted link
</commit_message>
<xml_diff>
--- a/Capital_One_job( php_developer ).xlsx
+++ b/Capital_One_job( php_developer ).xlsx
@@ -112,83 +112,83 @@
     <t>Richmond, VA</t>
   </si>
   <si>
-    <t>/job/mclean/executive-assistant-corporate-development/1732/84767072784</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-strategic-partnership-development/1732/84767067904</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-product-management-developer-experience/1732/84767070880</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-product-management-developer-experience/1732/84767070160</t>
-  </si>
-  <si>
-    <t>/job/bengaluru/principal-associate-software-full-stack-developer/1732/84767015648</t>
-  </si>
-  <si>
-    <t>/job/chicago/senior-manager-software-engineering-mobile-development/1732/84767015360</t>
-  </si>
-  <si>
-    <t>/job/mclean/sr-distinguished-engineer-developer-enablement/1732/84767014480</t>
-  </si>
-  <si>
-    <t>/job/mclean/sr-distinguished-engineer-developer-enablement/1732/84767012960</t>
-  </si>
-  <si>
-    <t>/job/new-york/sr-associate-business-development-luxury-travel/1732/84794185536</t>
-  </si>
-  <si>
-    <t>/job/plano/distinguished-engineer-developer-experience-platform-modernization/1732/84767014432</t>
-  </si>
-  <si>
-    <t>/job/plano/distinguished-engineer-developer-experience-platform-modernization/1732/84767013280</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-strategic-business-consultant-enterprise-learning-and-development/1732/84768133024</t>
-  </si>
-  <si>
-    <t>/job/new-york/administrative-support-assistant-iii-ep-tech-developer-experience/1732/84767071184</t>
-  </si>
-  <si>
-    <t>/job/richmond/director-product-management-developer-experience-api-platforms/1732/84767049648</t>
-  </si>
-  <si>
-    <t>/job/mclean/director-product-management-developer-experience-network-observability/1732/84767013840</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-strategic-business-learning-consultant-enterprise-learning-and-development/1732/84767014352</t>
-  </si>
-  <si>
-    <t>/job/richmond/director-client-development-capital-one-ad-solutions-remote/1732/84767013392</t>
-  </si>
-  <si>
-    <t>/job/mclean/sr-director-product-management-developer-experience-quality-assurance/1732/84766996288</t>
-  </si>
-  <si>
-    <t>/job/richmond/director-business-development-databolt-capital-one-software-remote/1732/84768143840</t>
-  </si>
-  <si>
-    <t>/job/richmond/senior-manager-client-development-capital-one-ad-solutions-remote/1732/84768133232</t>
-  </si>
-  <si>
-    <t>/job/richmond/director-business-development-databolt-capital-one-software-remote/1732/84767057632</t>
-  </si>
-  <si>
-    <t>/job/mclean/manager-strategic-business-learning-consultant-enterprise-learning-and-development-risk/1732/84767014656</t>
-  </si>
-  <si>
-    <t>/job/mclean/sr-director-product-management-developer-experience-operational-intelligence-and-observability/1732/84767066560</t>
-  </si>
-  <si>
-    <t>/job/richmond/director-client-development-capital-one-ad-solutions-travel-partnerships-remote/1732/84767065728</t>
+    <t>https://www.capitalonecareers.com/job/mclean/executive-assistant-corporate-development/1732/84767072784</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-strategic-partnership-development/1732/84767067904</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-product-management-developer-experience/1732/84767070880</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-product-management-developer-experience/1732/84767070160</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/bengaluru/principal-associate-software-full-stack-developer/1732/84767015648</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/chicago/senior-manager-software-engineering-mobile-development/1732/84767015360</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/sr-distinguished-engineer-developer-enablement/1732/84767014480</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/sr-distinguished-engineer-developer-enablement/1732/84767012960</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/new-york/sr-associate-business-development-luxury-travel/1732/84794185536</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/plano/distinguished-engineer-developer-experience-platform-modernization/1732/84767014432</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/plano/distinguished-engineer-developer-experience-platform-modernization/1732/84767013280</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-strategic-business-consultant-enterprise-learning-and-development/1732/84768133024</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/new-york/administrative-support-assistant-iii-ep-tech-developer-experience/1732/84767071184</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/director-product-management-developer-experience-api-platforms/1732/84767049648</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/director-product-management-developer-experience-network-observability/1732/84767013840</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-strategic-business-learning-consultant-enterprise-learning-and-development/1732/84767014352</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/director-client-development-capital-one-ad-solutions-remote/1732/84767013392</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/sr-director-product-management-developer-experience-quality-assurance/1732/84766996288</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/director-business-development-databolt-capital-one-software-remote/1732/84768143840</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/senior-manager-client-development-capital-one-ad-solutions-remote/1732/84768133232</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/director-business-development-databolt-capital-one-software-remote/1732/84767057632</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/manager-strategic-business-learning-consultant-enterprise-learning-and-development-risk/1732/84767014656</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/mclean/sr-director-product-management-developer-experience-operational-intelligence-and-observability/1732/84767066560</t>
+  </si>
+  <si>
+    <t>https://www.capitalonecareers.com/job/richmond/director-client-development-capital-one-ad-solutions-travel-partnerships-remote/1732/84767065728</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,16 +244,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,7 +582,7 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -583,7 +596,7 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -597,7 +610,7 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -611,7 +624,7 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -625,7 +638,7 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -639,7 +652,7 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -653,7 +666,7 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -667,7 +680,7 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -681,7 +694,7 @@
       <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -695,7 +708,7 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -709,7 +722,7 @@
       <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -723,7 +736,7 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -737,7 +750,7 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -751,7 +764,7 @@
       <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -765,7 +778,7 @@
       <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -779,7 +792,7 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -793,7 +806,7 @@
       <c r="C18" t="s">
         <v>31</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -807,7 +820,7 @@
       <c r="C19" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -821,7 +834,7 @@
       <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -835,7 +848,7 @@
       <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -849,7 +862,7 @@
       <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -863,7 +876,7 @@
       <c r="C23" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -877,7 +890,7 @@
       <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -891,11 +904,37 @@
       <c r="C25" t="s">
         <v>31</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>